<commit_message>
Latest changes added,final project
</commit_message>
<xml_diff>
--- a/FinalProject/src/main/java/Resources/Test_Data.xlsx
+++ b/FinalProject/src/main/java/Resources/Test_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/38ee590834e4dbc6/Desktop/JAVA_TRAINING/TestData/FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{55D3C0C0-B631-4764-B9E0-1F90781C3F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BA7129A-E34A-42F8-8068-CFA602EA33ED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{3AC3086D-E9CE-4017-9C70-B28C2905ADF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="9" xr2:uid="{54D12617-C092-4A06-B96E-449AEA46C3A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="10" xr2:uid="{54D12617-C092-4A06-B96E-449AEA46C3A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Manage_Pages" sheetId="8" r:id="rId8"/>
     <sheet name="Manage_News" sheetId="9" r:id="rId9"/>
     <sheet name="Manage_Slider" sheetId="10" r:id="rId10"/>
+    <sheet name="Mobile_Slider" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Dashboard | 7rmart supermarket</t>
   </si>
@@ -145,6 +146,21 @@
   </si>
   <si>
     <t>https://groceryapp.uniqassosiates.com/admin/home</t>
+  </si>
+  <si>
+    <t>Table headers</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Edit button</t>
+  </si>
+  <si>
+    <t>Delete button</t>
   </si>
 </sst>
 </file>
@@ -208,10 +224,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -541,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE8B02E-9829-43F5-BA56-881AFDBF559E}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,6 +579,58 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E45433-C82C-4B62-BAD6-0D60F25A5C37}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC3B7B8-AA23-4A2F-B268-01C2840F3400}">
   <dimension ref="A1"/>

</xml_diff>